<commit_message>
Added metadata index processing
</commit_message>
<xml_diff>
--- a/minlp/Parameters.xlsx
+++ b/minlp/Parameters.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="9390" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="9390"/>
   </bookViews>
   <sheets>
-    <sheet name="Cost-Related" sheetId="1" r:id="rId1"/>
-    <sheet name="Capacity-Related" sheetId="2" r:id="rId2"/>
-    <sheet name="Inventory-Related" sheetId="3" r:id="rId3"/>
-    <sheet name="Time-Related" sheetId="4" r:id="rId4"/>
-    <sheet name="Bundle COmposition and PRicing" sheetId="5" r:id="rId5"/>
-    <sheet name="Reservation Price Parameters" sheetId="6" r:id="rId6"/>
+    <sheet name="Metadata" sheetId="7" r:id="rId1"/>
+    <sheet name="Cost-Related" sheetId="1" r:id="rId2"/>
+    <sheet name="Capacity-Related" sheetId="2" r:id="rId3"/>
+    <sheet name="Inventory-Related" sheetId="3" r:id="rId4"/>
+    <sheet name="Time-Related" sheetId="4" r:id="rId5"/>
+    <sheet name="Bundle COmposition and PRicing" sheetId="5" r:id="rId6"/>
+    <sheet name="Reservation Price Parameters" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="73">
   <si>
     <t>VC_if</t>
   </si>
@@ -192,9 +193,6 @@
     <t>r=4</t>
   </si>
   <si>
-    <t>&lt;&gt;</t>
-  </si>
-  <si>
     <t>TCFW_jfw&amp;f=1</t>
   </si>
   <si>
@@ -238,6 +236,48 @@
   </si>
   <si>
     <t>k=6</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>RANGE</t>
+  </si>
+  <si>
+    <t>1-7</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>4-7</t>
+  </si>
+  <si>
+    <t>INDEX_METADATA</t>
   </si>
 </sst>
 </file>
@@ -316,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -352,6 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +665,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,10 +673,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q95"/>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +884,7 @@
     </row>
     <row r="14" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <f>B12+B11</f>
@@ -773,7 +897,7 @@
     </row>
     <row r="15" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <f>B11+B13</f>
@@ -786,7 +910,7 @@
     </row>
     <row r="16" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <f>B12+B13</f>
@@ -797,9 +921,9 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <f>B11+B12+B13</f>
@@ -810,7 +934,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -824,7 +948,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -840,7 +964,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -856,7 +980,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -872,9 +996,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23">
         <f>B21+B20</f>
@@ -889,9 +1013,9 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24">
         <f>B20+B22</f>
@@ -906,9 +1030,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25">
         <f>B21+B22</f>
@@ -923,9 +1047,9 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <f>B20+B21+B22</f>
@@ -940,9 +1064,9 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>37</v>
@@ -953,23 +1077,9 @@
       <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -982,23 +1092,9 @@
       <c r="D29">
         <v>0.7</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29">
-        <v>0.7</v>
-      </c>
-      <c r="H29">
-        <v>0.5</v>
-      </c>
-      <c r="I29">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1011,23 +1107,9 @@
       <c r="D30">
         <v>0.75</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30">
-        <v>0.75</v>
-      </c>
-      <c r="H30">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I30">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
@@ -1040,1355 +1122,1504 @@
       <c r="D31">
         <v>0.65</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31">
-        <v>0.65</v>
-      </c>
-      <c r="H31">
-        <v>0.45</v>
-      </c>
-      <c r="I31">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32">
         <f>B30+B29</f>
         <v>1.05</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:I32" si="3">C30+C29</f>
+        <f t="shared" ref="C32:D32" si="3">C30+C29</f>
         <v>1.05</v>
       </c>
       <c r="D32">
         <f t="shared" si="3"/>
         <v>1.45</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="3"/>
-        <v>1.45</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="3"/>
-        <v>1.05</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="3"/>
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B33">
         <f>B29+B31</f>
         <v>0.95</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:I33" si="4">C29+C31</f>
+        <f t="shared" ref="C33:D33" si="4">C29+C31</f>
         <v>0.95</v>
       </c>
       <c r="D33">
         <f t="shared" si="4"/>
         <v>1.35</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="4"/>
-        <v>1.35</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="4"/>
-        <v>0.95</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="4"/>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34">
         <f>B30+B31</f>
         <v>1</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:I34" si="5">C30+C31</f>
+        <f t="shared" ref="C34:D34" si="5">C30+C31</f>
         <v>1</v>
       </c>
       <c r="D34">
         <f t="shared" si="5"/>
         <v>1.4</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="5"/>
-        <v>1.4</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <f>B29+B30+B31</f>
         <v>1.5</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:I35" si="6">C29+C30+C31</f>
+        <f t="shared" ref="C35:D35" si="6">C29+C30+C31</f>
         <v>1.5</v>
       </c>
       <c r="D35">
         <f t="shared" si="6"/>
         <v>2.1</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="6"/>
-        <v>2.1</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B38">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="C38">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D38">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E38">
-        <v>1.2</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38">
-        <v>1.2</v>
-      </c>
-      <c r="I38">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J38">
-        <v>0.9</v>
-      </c>
-      <c r="K38">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B39">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="C39">
-        <v>0.95</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D39">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E39">
-        <v>1.25</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39">
-        <v>1.25</v>
-      </c>
-      <c r="I39">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="J39">
-        <v>0.95</v>
-      </c>
-      <c r="K39">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B40">
-        <v>0.85</v>
+        <v>0.65</v>
       </c>
       <c r="C40">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="D40">
-        <v>1.05</v>
-      </c>
-      <c r="E40">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H40">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="I40">
-        <v>1.05</v>
-      </c>
-      <c r="J40">
-        <v>0.85</v>
-      </c>
-      <c r="K40">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.45</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41">
         <f>B39+B38</f>
-        <v>1.85</v>
+        <v>1.45</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:K41" si="7">C39+C38</f>
-        <v>1.85</v>
+        <f>C39+C38</f>
+        <v>1.05</v>
       </c>
       <c r="D41">
-        <f t="shared" si="7"/>
-        <v>2.25</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="7"/>
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G41" s="1" t="s">
+        <f>D39+D38</f>
+        <v>1.05</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="7"/>
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="7"/>
-        <v>2.25</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="7"/>
-        <v>1.85</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="7"/>
-        <v>1.85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="B42">
         <f>B38+B40</f>
-        <v>1.75</v>
+        <v>1.35</v>
       </c>
       <c r="C42">
-        <f t="shared" ref="C42:K42" si="8">C38+C40</f>
-        <v>1.75</v>
+        <f>C38+C40</f>
+        <v>0.95</v>
       </c>
       <c r="D42">
-        <f t="shared" si="8"/>
-        <v>2.1500000000000004</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="8"/>
-        <v>2.3499999999999996</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="8"/>
-        <v>2.3499999999999996</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="8"/>
-        <v>2.1500000000000004</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="8"/>
-        <v>1.75</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="8"/>
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <f>D38+D40</f>
+        <v>0.95</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43">
         <f>B39+B40</f>
-        <v>1.7999999999999998</v>
+        <v>1.4</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:K43" si="9">C39+C40</f>
-        <v>1.7999999999999998</v>
+        <f>C39+C40</f>
+        <v>1</v>
       </c>
       <c r="D43">
-        <f t="shared" si="9"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="9"/>
-        <v>2.4</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="9"/>
-        <v>2.4</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="9"/>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="9"/>
-        <v>1.7999999999999998</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="9"/>
-        <v>1.7999999999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+        <f>D39+D40</f>
+        <v>1</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44">
         <f>B38+B39+B40</f>
-        <v>2.7</v>
+        <v>2.1</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:K44" si="10">C38+C39+C40</f>
-        <v>2.7</v>
+        <f>C38+C39+C40</f>
+        <v>1.5</v>
       </c>
       <c r="D44">
-        <f t="shared" si="10"/>
-        <v>3.3</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="10"/>
-        <v>3.6</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="10"/>
-        <v>3.6</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="10"/>
-        <v>3.3</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="10"/>
-        <v>2.7</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="10"/>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <f>D38+D39+D40</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J46" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K46" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L46" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M46" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N46" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="O46" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="P46" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q46" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B47">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="C47">
-        <v>0.2</v>
+        <v>0.9</v>
       </c>
       <c r="D47">
-        <v>0.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E47">
-        <v>0.4</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H47">
-        <v>0.3</v>
-      </c>
-      <c r="I47">
-        <v>0.2</v>
-      </c>
-      <c r="J47">
-        <v>0.2</v>
-      </c>
-      <c r="K47">
-        <v>0.3</v>
-      </c>
-      <c r="L47" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M47" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N47">
-        <v>0.4</v>
-      </c>
-      <c r="O47">
-        <v>0.3</v>
-      </c>
-      <c r="P47">
-        <v>0.2</v>
-      </c>
-      <c r="Q47">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1.2</v>
+      </c>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B48">
-        <v>0.25</v>
+        <v>0.95</v>
       </c>
       <c r="C48">
-        <v>0.25</v>
+        <v>0.95</v>
       </c>
       <c r="D48">
-        <v>0.35</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E48">
-        <v>0.45</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H48">
-        <v>0.35</v>
-      </c>
-      <c r="I48">
-        <v>0.25</v>
-      </c>
-      <c r="J48">
-        <v>0.25</v>
-      </c>
-      <c r="K48">
-        <v>0.35</v>
-      </c>
-      <c r="L48" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N48">
-        <v>0.45</v>
-      </c>
-      <c r="O48">
-        <v>0.35</v>
-      </c>
-      <c r="P48">
-        <v>0.25</v>
-      </c>
-      <c r="Q48">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1.25</v>
+      </c>
+      <c r="F48" s="9"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B49">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="C49">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="D49">
-        <v>0.25</v>
+        <v>1.05</v>
       </c>
       <c r="E49">
-        <v>0.35</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49">
-        <v>0.35</v>
-      </c>
-      <c r="I49">
-        <v>0.15</v>
-      </c>
-      <c r="J49">
-        <v>0.15</v>
-      </c>
-      <c r="K49">
-        <v>0.25</v>
-      </c>
-      <c r="L49" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N49">
-        <v>0.35</v>
-      </c>
-      <c r="O49">
-        <v>0.25</v>
-      </c>
-      <c r="P49">
-        <v>0.15</v>
-      </c>
-      <c r="Q49">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F49" s="9"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <f>B48+B47</f>
+        <v>1.85</v>
+      </c>
+      <c r="C50">
+        <f>C48+C47</f>
+        <v>1.85</v>
+      </c>
+      <c r="D50">
+        <f>D48+D47</f>
+        <v>2.25</v>
+      </c>
+      <c r="E50">
+        <f t="shared" ref="E50:K50" si="7">E48+E47</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <f>B47+B49</f>
+        <v>1.75</v>
+      </c>
+      <c r="C51">
+        <f>C47+C49</f>
+        <v>1.75</v>
+      </c>
+      <c r="D51">
+        <f>D47+D49</f>
+        <v>2.1500000000000004</v>
+      </c>
+      <c r="E51">
+        <f t="shared" ref="E51:K51" si="8">E47+E49</f>
+        <v>2.3499999999999996</v>
+      </c>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <f>B48+B49</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="C52">
+        <f>C48+C49</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="D52">
+        <f>D48+D49</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E52">
+        <f t="shared" ref="E52:K52" si="9">E48+E49</f>
+        <v>2.4</v>
+      </c>
+      <c r="F52" s="9"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <f>B47+B48+B49</f>
+        <v>2.7</v>
+      </c>
+      <c r="C53">
+        <f>C47+C48+C49</f>
+        <v>2.7</v>
+      </c>
+      <c r="D53">
+        <f>D47+D48+D49</f>
+        <v>3.3</v>
+      </c>
+      <c r="E53">
+        <f t="shared" ref="E53:K53" si="10">E47+E48+E49</f>
+        <v>3.6</v>
+      </c>
+      <c r="F53" s="9"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56">
+        <v>1.2</v>
+      </c>
+      <c r="C56">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D56">
+        <v>0.9</v>
+      </c>
+      <c r="E56">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57">
+        <v>1.25</v>
+      </c>
+      <c r="C57">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D57">
+        <v>0.95</v>
+      </c>
+      <c r="E57">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C58">
+        <v>1.05</v>
+      </c>
+      <c r="D58">
+        <v>0.85</v>
+      </c>
+      <c r="E58">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59">
+        <f>B57+B56</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C59">
+        <f>C57+C56</f>
+        <v>2.25</v>
+      </c>
+      <c r="D59">
+        <f>D57+D56</f>
+        <v>1.85</v>
+      </c>
+      <c r="E59">
+        <f>E57+E56</f>
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60">
+        <f>B56+B58</f>
+        <v>2.3499999999999996</v>
+      </c>
+      <c r="C60">
+        <f>C56+C58</f>
+        <v>2.1500000000000004</v>
+      </c>
+      <c r="D60">
+        <f>D56+D58</f>
+        <v>1.75</v>
+      </c>
+      <c r="E60">
+        <f>E56+E58</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61">
+        <f>B57+B58</f>
+        <v>2.4</v>
+      </c>
+      <c r="C61">
+        <f>C57+C58</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D61">
+        <f>D57+D58</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E61">
+        <f>E57+E58</f>
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62">
+        <f>B56+B57+B58</f>
+        <v>3.6</v>
+      </c>
+      <c r="C62">
+        <f>C56+C57+C58</f>
+        <v>3.3</v>
+      </c>
+      <c r="D62">
+        <f>D56+D57+D58</f>
+        <v>2.7</v>
+      </c>
+      <c r="E62">
+        <f>E56+E57+E58</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" s="9"/>
+      <c r="L64" s="9"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65">
+        <v>0.2</v>
+      </c>
+      <c r="C65">
+        <v>0.2</v>
+      </c>
+      <c r="D65">
+        <v>0.3</v>
+      </c>
+      <c r="E65">
+        <v>0.4</v>
+      </c>
+      <c r="F65" s="9"/>
+      <c r="L65" s="9"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66">
+        <v>0.25</v>
+      </c>
+      <c r="C66">
+        <v>0.25</v>
+      </c>
+      <c r="D66">
+        <v>0.35</v>
+      </c>
+      <c r="E66">
         <v>0.45</v>
       </c>
-      <c r="C50">
-        <f t="shared" ref="C50:Q50" si="11">C48+C47</f>
+      <c r="F66" s="9"/>
+      <c r="L66" s="9"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67">
+        <v>0.15</v>
+      </c>
+      <c r="C67">
+        <v>0.15</v>
+      </c>
+      <c r="D67">
+        <v>0.25</v>
+      </c>
+      <c r="E67">
+        <v>0.35</v>
+      </c>
+      <c r="F67" s="9"/>
+      <c r="L67" s="9"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68">
+        <f>B66+B65</f>
         <v>0.45</v>
       </c>
-      <c r="D50">
+      <c r="C68">
+        <f t="shared" ref="C68:Q68" si="11">C66+C65</f>
+        <v>0.45</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="11"/>
         <v>0.64999999999999991</v>
       </c>
-      <c r="E50">
+      <c r="E68">
         <f t="shared" si="11"/>
         <v>0.85000000000000009</v>
       </c>
-      <c r="F50" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G50" s="1" t="s">
+      <c r="F68" s="9"/>
+      <c r="L68" s="9"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H50">
-        <f t="shared" si="11"/>
-        <v>0.64999999999999991</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="11"/>
-        <v>0.45</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="11"/>
-        <v>0.45</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="11"/>
-        <v>0.64999999999999991</v>
-      </c>
-      <c r="L50" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N50">
-        <f t="shared" si="11"/>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="O50">
-        <f t="shared" si="11"/>
-        <v>0.64999999999999991</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="11"/>
-        <v>0.45</v>
-      </c>
-      <c r="Q50">
-        <f t="shared" si="11"/>
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51">
-        <f>B47+B49</f>
+      <c r="B69">
+        <f>B65+B67</f>
         <v>0.35</v>
       </c>
-      <c r="C51">
-        <f t="shared" ref="C51:Q51" si="12">C47+C49</f>
+      <c r="C69">
+        <f t="shared" ref="C69:Q69" si="12">C65+C67</f>
         <v>0.35</v>
       </c>
-      <c r="D51">
+      <c r="D69">
         <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="E51">
+      <c r="E69">
         <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
-      <c r="F51" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="12"/>
-        <v>0.64999999999999991</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="12"/>
-        <v>0.35</v>
-      </c>
-      <c r="J51">
-        <f t="shared" si="12"/>
-        <v>0.35</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="12"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="L51" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N51">
-        <f t="shared" si="12"/>
-        <v>0.75</v>
-      </c>
-      <c r="O51">
-        <f t="shared" si="12"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="P51">
-        <f t="shared" si="12"/>
-        <v>0.35</v>
-      </c>
-      <c r="Q51">
-        <f t="shared" si="12"/>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52">
-        <f>B48+B49</f>
+      <c r="F69" s="9"/>
+      <c r="L69" s="9"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70">
+        <f>B66+B67</f>
         <v>0.4</v>
       </c>
-      <c r="C52">
-        <f t="shared" ref="C52:Q52" si="13">C48+C49</f>
+      <c r="C70">
+        <f t="shared" ref="C70:Q70" si="13">C66+C67</f>
         <v>0.4</v>
       </c>
-      <c r="D52">
+      <c r="D70">
         <f t="shared" si="13"/>
         <v>0.6</v>
       </c>
-      <c r="E52">
+      <c r="E70">
         <f t="shared" si="13"/>
         <v>0.8</v>
       </c>
-      <c r="F52" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="13"/>
-        <v>0.7</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="13"/>
-        <v>0.4</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="13"/>
-        <v>0.4</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="13"/>
+      <c r="F70" s="9"/>
+      <c r="L70" s="9"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B71">
+        <f>B65+B66+B67</f>
         <v>0.6</v>
       </c>
-      <c r="L52" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="13"/>
-        <v>0.8</v>
-      </c>
-      <c r="O52">
-        <f t="shared" si="13"/>
+      <c r="C71">
+        <f t="shared" ref="C71:Q71" si="14">C65+C66+C67</f>
         <v>0.6</v>
       </c>
-      <c r="P52">
-        <f t="shared" si="13"/>
-        <v>0.4</v>
-      </c>
-      <c r="Q52">
-        <f t="shared" si="13"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <f>B47+B48+B49</f>
-        <v>0.6</v>
-      </c>
-      <c r="C53">
-        <f t="shared" ref="C53:Q53" si="14">C47+C48+C49</f>
-        <v>0.6</v>
-      </c>
-      <c r="D53">
+      <c r="D71">
         <f t="shared" si="14"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="E53">
+      <c r="E71">
         <f t="shared" si="14"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="F53" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G53" s="1" t="s">
+      <c r="F71" s="9"/>
+      <c r="L71" s="9"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="1"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="1"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F73" s="9"/>
+      <c r="G73" s="1"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74">
+        <v>0.3</v>
+      </c>
+      <c r="C74">
+        <v>0.2</v>
+      </c>
+      <c r="D74">
+        <v>0.2</v>
+      </c>
+      <c r="E74">
+        <v>0.3</v>
+      </c>
+      <c r="F74" s="9"/>
+      <c r="G74" s="1"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75">
+        <v>0.35</v>
+      </c>
+      <c r="C75">
+        <v>0.25</v>
+      </c>
+      <c r="D75">
+        <v>0.25</v>
+      </c>
+      <c r="E75">
+        <v>0.35</v>
+      </c>
+      <c r="F75" s="9"/>
+      <c r="G75" s="1"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="1"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76">
+        <v>0.35</v>
+      </c>
+      <c r="C76">
+        <v>0.15</v>
+      </c>
+      <c r="D76">
+        <v>0.15</v>
+      </c>
+      <c r="E76">
+        <v>0.25</v>
+      </c>
+      <c r="F76" s="9"/>
+      <c r="G76" s="1"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="1"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77">
+        <f>B75+B74</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="C77">
+        <f>C75+C74</f>
+        <v>0.45</v>
+      </c>
+      <c r="D77">
+        <f>D75+D74</f>
+        <v>0.45</v>
+      </c>
+      <c r="E77">
+        <f>E75+E74</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="F77" s="9"/>
+      <c r="G77" s="1"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="1"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B78">
+        <f>B74+B76</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="C78">
+        <f>C74+C76</f>
+        <v>0.35</v>
+      </c>
+      <c r="D78">
+        <f>D74+D76</f>
+        <v>0.35</v>
+      </c>
+      <c r="E78">
+        <f>E74+E76</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F78" s="9"/>
+      <c r="G78" s="1"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="1"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H53">
-        <f t="shared" si="14"/>
+      <c r="B79">
+        <f>B75+B76</f>
+        <v>0.7</v>
+      </c>
+      <c r="C79">
+        <f>C75+C76</f>
+        <v>0.4</v>
+      </c>
+      <c r="D79">
+        <f>D75+D76</f>
+        <v>0.4</v>
+      </c>
+      <c r="E79">
+        <f>E75+E76</f>
+        <v>0.6</v>
+      </c>
+      <c r="F79" s="9"/>
+      <c r="G79" s="1"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="1"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B80">
+        <f>B74+B75+B76</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="I53">
-        <f t="shared" si="14"/>
+      <c r="C80">
+        <f>C74+C75+C76</f>
         <v>0.6</v>
       </c>
-      <c r="J53">
-        <f t="shared" si="14"/>
+      <c r="D80">
+        <f>D74+D75+D76</f>
         <v>0.6</v>
       </c>
-      <c r="K53">
-        <f t="shared" si="14"/>
+      <c r="E80">
+        <f>E74+E75+E76</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="L53" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M53" s="1" t="s">
+      <c r="F80" s="9"/>
+      <c r="G80" s="1"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="1"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="1"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="1"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F82" s="9"/>
+      <c r="G82" s="1"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B83">
+        <v>0.4</v>
+      </c>
+      <c r="C83">
+        <v>0.3</v>
+      </c>
+      <c r="D83">
+        <v>0.2</v>
+      </c>
+      <c r="E83">
+        <v>0.2</v>
+      </c>
+      <c r="F83" s="9"/>
+      <c r="G83" s="1"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="1"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84">
+        <v>0.45</v>
+      </c>
+      <c r="C84">
+        <v>0.35</v>
+      </c>
+      <c r="D84">
+        <v>0.25</v>
+      </c>
+      <c r="E84">
+        <v>0.25</v>
+      </c>
+      <c r="F84" s="9"/>
+      <c r="G84" s="1"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="1"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85">
+        <v>0.35</v>
+      </c>
+      <c r="C85">
+        <v>0.25</v>
+      </c>
+      <c r="D85">
+        <v>0.15</v>
+      </c>
+      <c r="E85">
+        <v>0.15</v>
+      </c>
+      <c r="F85" s="9"/>
+      <c r="G85" s="1"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="1"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B86">
+        <f>B84+B83</f>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="C86">
+        <f>C84+C83</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="D86">
+        <f>D84+D83</f>
+        <v>0.45</v>
+      </c>
+      <c r="E86">
+        <f>E84+E83</f>
+        <v>0.45</v>
+      </c>
+      <c r="F86" s="9"/>
+      <c r="G86" s="1"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="1"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B87">
+        <f>B83+B85</f>
+        <v>0.75</v>
+      </c>
+      <c r="C87">
+        <f>C83+C85</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D87">
+        <f>D83+D85</f>
+        <v>0.35</v>
+      </c>
+      <c r="E87">
+        <f>E83+E85</f>
+        <v>0.35</v>
+      </c>
+      <c r="F87" s="9"/>
+      <c r="G87" s="1"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="1"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N53">
-        <f t="shared" si="14"/>
+      <c r="B88">
+        <f>B84+B85</f>
+        <v>0.8</v>
+      </c>
+      <c r="C88">
+        <f>C84+C85</f>
+        <v>0.6</v>
+      </c>
+      <c r="D88">
+        <f>D84+D85</f>
+        <v>0.4</v>
+      </c>
+      <c r="E88">
+        <f>E84+E85</f>
+        <v>0.4</v>
+      </c>
+      <c r="F88" s="9"/>
+      <c r="G88" s="1"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="1"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B89">
+        <f>B83+B84+B85</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="O53">
-        <f t="shared" si="14"/>
+      <c r="C89">
+        <f>C83+C84+C85</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="P53">
-        <f t="shared" si="14"/>
+      <c r="D89">
+        <f>D83+D84+D85</f>
         <v>0.6</v>
       </c>
-      <c r="Q53">
-        <f t="shared" si="14"/>
+      <c r="E89">
+        <f>E83+E84+E85</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="F89" s="9"/>
+      <c r="G89" s="1"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="1"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="1"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="1"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B56">
+      <c r="B92">
         <v>3.5</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B57">
+      <c r="B93">
         <v>3.5</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B58">
+      <c r="B94">
         <v>3.5</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B59">
+      <c r="B95">
         <v>3.5</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B98">
+        <v>50000</v>
+      </c>
+      <c r="C98">
+        <v>50000</v>
+      </c>
+      <c r="D98">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B99">
+        <v>40000</v>
+      </c>
+      <c r="C99">
+        <v>40000</v>
+      </c>
+      <c r="D99">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B62">
-        <v>50000</v>
-      </c>
-      <c r="C62">
-        <v>50000</v>
-      </c>
-      <c r="D62">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="B100">
+        <v>45000</v>
+      </c>
+      <c r="C100">
+        <v>45000</v>
+      </c>
+      <c r="D100">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B63">
-        <v>40000</v>
-      </c>
-      <c r="C63">
-        <v>40000</v>
-      </c>
-      <c r="D63">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B64">
-        <v>45000</v>
-      </c>
-      <c r="C64">
-        <v>45000</v>
-      </c>
-      <c r="D64">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="B101">
+        <v>52000</v>
+      </c>
+      <c r="C101">
+        <v>52000</v>
+      </c>
+      <c r="D101">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B65">
-        <v>52000</v>
-      </c>
-      <c r="C65">
-        <v>52000</v>
-      </c>
-      <c r="D65">
-        <v>52000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="1" t="s">
+      <c r="B104">
+        <v>30000</v>
+      </c>
+      <c r="C104">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B105">
+        <v>20000</v>
+      </c>
+      <c r="C105">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B106">
+        <v>25000</v>
+      </c>
+      <c r="C106">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B107">
+        <v>32000</v>
+      </c>
+      <c r="C107">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B110">
+        <v>500</v>
+      </c>
+      <c r="C110">
+        <v>500</v>
+      </c>
+      <c r="D110">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B111">
+        <v>500</v>
+      </c>
+      <c r="C111">
+        <v>500</v>
+      </c>
+      <c r="D111">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B112">
+        <v>500</v>
+      </c>
+      <c r="C112">
+        <v>500</v>
+      </c>
+      <c r="D112">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B113">
+        <v>500</v>
+      </c>
+      <c r="C113">
+        <v>500</v>
+      </c>
+      <c r="D113">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B116">
+        <v>300</v>
+      </c>
+      <c r="C116">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B117">
+        <v>300</v>
+      </c>
+      <c r="C117">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B68">
-        <v>30000</v>
-      </c>
-      <c r="C68">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="B118">
+        <v>300</v>
+      </c>
+      <c r="C118">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B69">
-        <v>20000</v>
-      </c>
-      <c r="C69">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70">
-        <v>25000</v>
-      </c>
-      <c r="C70">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="B119">
+        <v>300</v>
+      </c>
+      <c r="C119">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B71">
-        <v>32000</v>
-      </c>
-      <c r="C71">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>7</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="B122">
+        <v>12.8</v>
+      </c>
+      <c r="C122">
+        <v>12.8</v>
+      </c>
+      <c r="D122">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B123">
+        <v>10.5</v>
+      </c>
+      <c r="C123">
+        <v>10.5</v>
+      </c>
+      <c r="D123">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B74">
-        <v>500</v>
-      </c>
-      <c r="C74">
-        <v>500</v>
-      </c>
-      <c r="D74">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="B124">
+        <v>11.5</v>
+      </c>
+      <c r="C124">
+        <v>11.5</v>
+      </c>
+      <c r="D124">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B75">
-        <v>500</v>
-      </c>
-      <c r="C75">
-        <v>500</v>
-      </c>
-      <c r="D75">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B76">
-        <v>500</v>
-      </c>
-      <c r="C76">
-        <v>500</v>
-      </c>
-      <c r="D76">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="B125">
+        <v>16.8</v>
+      </c>
+      <c r="C125">
+        <v>16.8</v>
+      </c>
+      <c r="D125">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>10</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B77">
-        <v>500</v>
-      </c>
-      <c r="C77">
-        <v>500</v>
-      </c>
-      <c r="D77">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>8</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="B128">
+        <v>12.5</v>
+      </c>
+      <c r="C128">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B80">
-        <v>300</v>
-      </c>
-      <c r="C80">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="B130">
+        <v>11</v>
+      </c>
+      <c r="C130">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B81">
-        <v>300</v>
-      </c>
-      <c r="C81">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82">
-        <v>300</v>
-      </c>
-      <c r="C82">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B83">
-        <v>300</v>
-      </c>
-      <c r="C83">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>9</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B86">
-        <v>12.8</v>
-      </c>
-      <c r="C86">
-        <v>12.8</v>
-      </c>
-      <c r="D86">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B87">
-        <v>10.5</v>
-      </c>
-      <c r="C87">
-        <v>10.5</v>
-      </c>
-      <c r="D87">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B88">
-        <v>11.5</v>
-      </c>
-      <c r="C88">
-        <v>11.5</v>
-      </c>
-      <c r="D88">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B89">
-        <v>16.8</v>
-      </c>
-      <c r="C89">
-        <v>16.8</v>
-      </c>
-      <c r="D89">
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B92">
-        <v>12.5</v>
-      </c>
-      <c r="C92">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B93">
-        <v>10</v>
-      </c>
-      <c r="C93">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B94">
-        <v>11</v>
-      </c>
-      <c r="C94">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B95">
+      <c r="B131">
         <v>16.5</v>
       </c>
-      <c r="C95">
+      <c r="C131">
         <v>16.5</v>
       </c>
     </row>
@@ -2397,12 +2628,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,7 +2751,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>2800</v>
@@ -2534,7 +2765,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>2300</v>
@@ -2548,7 +2779,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18">
         <v>2550</v>
@@ -2562,7 +2793,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19">
         <v>2100</v>
@@ -2587,7 +2818,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22">
         <v>3000</v>
@@ -2598,7 +2829,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>2500</v>
@@ -2609,7 +2840,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>2750</v>
@@ -2620,7 +2851,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25">
         <v>2300</v>
@@ -2634,7 +2865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -2778,7 +3009,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>1.5</v>
@@ -2786,7 +3017,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>1.5</v>
@@ -2794,7 +3025,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17">
         <v>1.5</v>
@@ -2802,7 +3033,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2814,7 +3045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -3027,7 +3258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -3051,16 +3282,16 @@
         <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3154,11 +3385,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added constraints, missing index check
</commit_message>
<xml_diff>
--- a/minlp/Parameters.xlsx
+++ b/minlp/Parameters.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="80">
   <si>
     <t>VC_if</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>10000000</t>
+  </si>
+  <si>
+    <t>LE1</t>
+  </si>
+  <si>
+    <t>0.999</t>
   </si>
 </sst>
 </file>
@@ -683,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,16 +697,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
@@ -774,6 +780,14 @@
       </c>
       <c r="B10" s="12" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -787,7 +801,7 @@
   <dimension ref="A1:M132"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,11 +916,10 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C12">
-        <f>B12</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -914,11 +927,10 @@
         <v>24</v>
       </c>
       <c r="B13">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C18" si="0">B13</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -926,11 +938,10 @@
         <v>25</v>
       </c>
       <c r="B14">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -939,11 +950,11 @@
       </c>
       <c r="B15">
         <f>B13+B12</f>
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
+        <f t="shared" ref="C15:C18" si="0">B15</f>
+        <v>0.35</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -952,11 +963,11 @@
       </c>
       <c r="B16">
         <f>B12+B14</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -965,11 +976,11 @@
       </c>
       <c r="B17">
         <f>B13+B14</f>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -978,11 +989,11 @@
       </c>
       <c r="B18">
         <f>B12+B13+B14</f>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1004,15 +1015,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="C21">
-        <f>B21</f>
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="D21">
-        <f>B21</f>
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1020,15 +1029,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:C27" si="1">B22</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:D27" si="2">B22</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1036,15 +1043,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1053,15 +1058,15 @@
       </c>
       <c r="B24">
         <f>B22+B21</f>
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
-        <v>0.35</v>
+        <f t="shared" ref="C24:C27" si="1">B24</f>
+        <v>0.45</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
-        <v>0.35</v>
+        <f t="shared" ref="D24:D27" si="2">B24</f>
+        <v>0.45</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1070,15 +1075,15 @@
       </c>
       <c r="B25">
         <f>B21+B23</f>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1087,15 +1092,15 @@
       </c>
       <c r="B26">
         <f>B22+B23</f>
-        <v>0.45</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1104,15 +1109,15 @@
       </c>
       <c r="B27">
         <f>B21+B22+B23</f>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="D27">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,13 +2573,13 @@
         <v>51</v>
       </c>
       <c r="B123">
-        <v>12.8</v>
+        <v>1.8</v>
       </c>
       <c r="C123">
-        <v>12.8</v>
+        <v>1.8</v>
       </c>
       <c r="D123">
-        <v>12.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2582,13 +2587,13 @@
         <v>49</v>
       </c>
       <c r="B124">
-        <v>10.5</v>
+        <v>1.5</v>
       </c>
       <c r="C124">
-        <v>10.5</v>
+        <v>1.5</v>
       </c>
       <c r="D124">
-        <v>10.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2596,13 +2601,13 @@
         <v>52</v>
       </c>
       <c r="B125">
-        <v>11.5</v>
+        <v>2.5</v>
       </c>
       <c r="C125">
-        <v>11.5</v>
+        <v>2.5</v>
       </c>
       <c r="D125">
-        <v>11.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2610,13 +2615,13 @@
         <v>50</v>
       </c>
       <c r="B126">
-        <v>16.8</v>
+        <v>1.8</v>
       </c>
       <c r="C126">
-        <v>16.8</v>
+        <v>1.8</v>
       </c>
       <c r="D126">
-        <v>16.8</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2635,10 +2640,10 @@
         <v>51</v>
       </c>
       <c r="B129">
-        <v>12.5</v>
+        <v>1.5</v>
       </c>
       <c r="C129">
-        <v>12.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2646,10 +2651,10 @@
         <v>49</v>
       </c>
       <c r="B130">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C130">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2657,10 +2662,10 @@
         <v>52</v>
       </c>
       <c r="B131">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C131">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2668,10 +2673,10 @@
         <v>50</v>
       </c>
       <c r="B132">
-        <v>16.5</v>
+        <v>1.5</v>
       </c>
       <c r="C132">
-        <v>16.5</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +2925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -3101,7 +3106,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3170,16 +3175,16 @@
         <v>29</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3187,16 +3192,16 @@
         <v>30</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3277,7 +3282,7 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3285,7 +3290,7 @@
         <v>35</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3293,7 +3298,7 @@
         <v>36</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3301,7 +3306,7 @@
         <v>37</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beginning of the end
</commit_message>
<xml_diff>
--- a/minlp/Parameters.xlsx
+++ b/minlp/Parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="465" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="11640" yWindow="465" windowWidth="20640" windowHeight="11760" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="7" r:id="rId1"/>
@@ -14,8 +14,9 @@
     <sheet name="Time-Related" sheetId="4" r:id="rId5"/>
     <sheet name="Bundle COmposition and PRicing" sheetId="5" r:id="rId6"/>
     <sheet name="Reservation Price Parameters" sheetId="8" r:id="rId7"/>
+    <sheet name="SP, alpha" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="91">
   <si>
     <t>VC_if</t>
   </si>
@@ -329,6 +330,12 @@
   </si>
   <si>
     <t>0.999</t>
+  </si>
+  <si>
+    <t>SP_jt</t>
+  </si>
+  <si>
+    <t>alpha_jt</t>
   </si>
 </sst>
 </file>
@@ -407,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -444,6 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,7 +724,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -726,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD12"/>
     </sheetView>
   </sheetViews>
@@ -827,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M132"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+    <sheetView topLeftCell="A7" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,12 +1287,12 @@
       </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="E37" s="9"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>39</v>
       </c>
@@ -1300,7 +1308,7 @@
       <c r="E38" s="9"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -1316,7 +1324,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1340,7 @@
       <c r="E40" s="9"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>25</v>
       </c>
@@ -1348,7 +1356,7 @@
       <c r="E41" s="9"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1367,7 +1375,7 @@
       <c r="E42" s="9"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1386,7 +1394,7 @@
       <c r="E43" s="9"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -1405,7 +1413,7 @@
       <c r="E44" s="9"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
@@ -1422,10 +1430,10 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>40</v>
       </c>
@@ -1443,7 +1451,7 @@
       </c>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
@@ -1461,7 +1469,7 @@
       </c>
       <c r="F48" s="9"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
@@ -1479,7 +1487,7 @@
       </c>
       <c r="F49" s="9"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +1505,7 @@
       </c>
       <c r="F50" s="9"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
@@ -1519,7 +1527,7 @@
       </c>
       <c r="F51" s="9"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
@@ -1541,7 +1549,7 @@
       </c>
       <c r="F52" s="9"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>46</v>
       </c>
@@ -1563,7 +1571,7 @@
       </c>
       <c r="F53" s="9"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>45</v>
       </c>
@@ -1585,7 +1593,7 @@
       </c>
       <c r="F54" s="9"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>41</v>
       </c>
@@ -1602,7 +1610,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>23</v>
       </c>
@@ -1619,7 +1627,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>24</v>
       </c>
@@ -1636,7 +1644,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>25</v>
       </c>
@@ -1653,7 +1661,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>47</v>
       </c>
@@ -1674,7 +1682,7 @@
         <v>1.85</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
@@ -1695,7 +1703,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>46</v>
       </c>
@@ -1716,7 +1724,7 @@
         <v>1.7999999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>45</v>
       </c>
@@ -1737,7 +1745,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>42</v>
       </c>
@@ -1756,7 +1764,7 @@
       <c r="F65" s="9"/>
       <c r="L65" s="9"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>23</v>
       </c>
@@ -1775,7 +1783,7 @@
       <c r="F66" s="9"/>
       <c r="L66" s="9"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>24</v>
       </c>
@@ -1794,7 +1802,7 @@
       <c r="F67" s="9"/>
       <c r="L67" s="9"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
@@ -1813,7 +1821,7 @@
       <c r="F68" s="9"/>
       <c r="L68" s="9"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>47</v>
       </c>
@@ -1836,7 +1844,7 @@
       <c r="F69" s="9"/>
       <c r="L69" s="9"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>48</v>
       </c>
@@ -1859,7 +1867,7 @@
       <c r="F70" s="9"/>
       <c r="L70" s="9"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>46</v>
       </c>
@@ -1882,7 +1890,7 @@
       <c r="F71" s="9"/>
       <c r="L71" s="9"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>45</v>
       </c>
@@ -1905,14 +1913,14 @@
       <c r="F72" s="9"/>
       <c r="L72" s="9"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="F73" s="9"/>
       <c r="G73" s="1"/>
       <c r="L73" s="9"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>43</v>
       </c>
@@ -1933,7 +1941,7 @@
       <c r="L74" s="9"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>23</v>
       </c>
@@ -1954,7 +1962,7 @@
       <c r="L75" s="9"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>24</v>
       </c>
@@ -1975,7 +1983,7 @@
       <c r="L76" s="9"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>25</v>
       </c>
@@ -1996,7 +2004,7 @@
       <c r="L77" s="9"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>47</v>
       </c>
@@ -2021,7 +2029,7 @@
       <c r="L78" s="9"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>48</v>
       </c>
@@ -2046,7 +2054,7 @@
       <c r="L79" s="9"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>46</v>
       </c>
@@ -2071,7 +2079,7 @@
       <c r="L80" s="9"/>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>45</v>
       </c>
@@ -2096,14 +2104,14 @@
       <c r="L81" s="9"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="F82" s="9"/>
       <c r="G82" s="1"/>
       <c r="L82" s="9"/>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>44</v>
       </c>
@@ -2124,7 +2132,7 @@
       <c r="L83" s="9"/>
       <c r="M83" s="1"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>23</v>
       </c>
@@ -2145,7 +2153,7 @@
       <c r="L84" s="9"/>
       <c r="M84" s="1"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>24</v>
       </c>
@@ -2166,7 +2174,7 @@
       <c r="L85" s="9"/>
       <c r="M85" s="1"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>25</v>
       </c>
@@ -2187,7 +2195,7 @@
       <c r="L86" s="9"/>
       <c r="M86" s="1"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>47</v>
       </c>
@@ -2212,7 +2220,7 @@
       <c r="L87" s="9"/>
       <c r="M87" s="1"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>48</v>
       </c>
@@ -2237,7 +2245,7 @@
       <c r="L88" s="9"/>
       <c r="M88" s="1"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>46</v>
       </c>
@@ -2262,7 +2270,7 @@
       <c r="L89" s="9"/>
       <c r="M89" s="1"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>45</v>
       </c>
@@ -2287,19 +2295,19 @@
       <c r="L90" s="9"/>
       <c r="M90" s="1"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="F91" s="9"/>
       <c r="G91" s="1"/>
       <c r="L91" s="9"/>
       <c r="M91" s="1"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>34</v>
       </c>
@@ -2307,7 +2315,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>35</v>
       </c>
@@ -2315,7 +2323,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>36</v>
       </c>
@@ -2323,7 +2331,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>37</v>
       </c>
@@ -2331,7 +2339,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -2345,7 +2353,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>51</v>
       </c>
@@ -2359,7 +2367,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>49</v>
       </c>
@@ -2373,7 +2381,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>52</v>
       </c>
@@ -2387,7 +2395,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>50</v>
       </c>
@@ -2401,7 +2409,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -2412,7 +2420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>51</v>
       </c>
@@ -2423,7 +2431,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>49</v>
       </c>
@@ -2434,7 +2442,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>52</v>
       </c>
@@ -2445,7 +2453,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>50</v>
       </c>
@@ -2456,7 +2464,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -2470,7 +2478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>51</v>
       </c>
@@ -2484,7 +2492,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>49</v>
       </c>
@@ -2498,7 +2506,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>52</v>
       </c>
@@ -2512,7 +2520,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>50</v>
       </c>
@@ -2526,7 +2534,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>7</v>
       </c>
@@ -2537,7 +2545,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>51</v>
       </c>
@@ -2548,7 +2556,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>49</v>
       </c>
@@ -2559,7 +2567,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>52</v>
       </c>
@@ -2570,7 +2578,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>50</v>
       </c>
@@ -2581,7 +2589,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -2595,7 +2603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>51</v>
       </c>
@@ -2609,7 +2617,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>49</v>
       </c>
@@ -2715,7 +2723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -3473,7 +3481,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3760,7 +3768,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -3786,12 +3794,12 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -3799,7 +3807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3807,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3815,12 +3823,521 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
       <c r="B34">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <f>B2/1.05</f>
+        <v>13.333333333333332</v>
+      </c>
+      <c r="M2">
+        <v>15</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <f>B3/1.05</f>
+        <v>15.238095238095237</v>
+      </c>
+      <c r="M3">
+        <v>17</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J7" si="0">B4/1.05</f>
+        <v>11.428571428571429</v>
+      </c>
+      <c r="M4">
+        <v>13</v>
+      </c>
+      <c r="N4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="M5">
+        <f>M2+M3</f>
+        <v>32</v>
+      </c>
+      <c r="N5">
+        <f>SQRT(N2^2+N3^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>26</v>
+      </c>
+      <c r="F6">
+        <v>26</v>
+      </c>
+      <c r="G6">
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>24.761904761904759</v>
+      </c>
+      <c r="M6">
+        <f>M2+M4</f>
+        <v>28</v>
+      </c>
+      <c r="N6">
+        <f>SQRT(N2^2+N4^2)</f>
+        <v>1.1180339887498949</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>28</v>
+      </c>
+      <c r="G7">
+        <v>28</v>
+      </c>
+      <c r="H7">
+        <v>28</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>26.666666666666664</v>
+      </c>
+      <c r="M7">
+        <f>M3+M4</f>
+        <v>30</v>
+      </c>
+      <c r="N7">
+        <f>SQRT(N4^2+N3^2)</f>
+        <v>2.0615528128088303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>42</v>
+      </c>
+      <c r="C8">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>42</v>
+      </c>
+      <c r="G8">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>42</v>
+      </c>
+      <c r="J8">
+        <f>B8/1.05</f>
+        <v>40</v>
+      </c>
+      <c r="M8">
+        <f>SUM(M2:M4)</f>
+        <v>45</v>
+      </c>
+      <c r="N8">
+        <f>SQRT(N2^2+N3^2+N4^2)</f>
+        <v>2.2912878474779199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>0.22</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.22</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0.22</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0.3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0.3</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17">
+        <v>0.22</v>
+      </c>
+      <c r="C17">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D17">
+        <v>0.22</v>
+      </c>
+      <c r="E17">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F17">
+        <v>0.22</v>
+      </c>
+      <c r="G17">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H17">
+        <v>0.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test long eval time
</commit_message>
<xml_diff>
--- a/minlp/Parameters.xlsx
+++ b/minlp/Parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="465" windowWidth="20640" windowHeight="11760" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="11640" yWindow="465" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="7" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="92">
   <si>
     <t>VC_if</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>alpha_jt</t>
+  </si>
+  <si>
+    <t>IntegralLimit</t>
   </si>
 </sst>
 </file>
@@ -724,7 +727,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,6 +826,14 @@
       </c>
       <c r="B12" s="12" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -3840,8 +3851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added all contingency except special
Added all contingency except special 2
</commit_message>
<xml_diff>
--- a/minlp/Parameters.xlsx
+++ b/minlp/Parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="465" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="11640" yWindow="465" windowWidth="20640" windowHeight="11760" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="7" r:id="rId1"/>
@@ -737,7 +737,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -747,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -3089,7 +3089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>2550</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>2750</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>50</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
@@ -3729,8 +3729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,7 +4061,7 @@
         <v>49</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>52</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>